<commit_message>
working hours adjusted and documentation enhanced
</commit_message>
<xml_diff>
--- a/dist-db-working-hours-janeczek-mair.xlsx
+++ b/dist-db-working-hours-janeczek-mair.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
   </bookViews>
   <sheets>
     <sheet name="Janeczek" sheetId="8" r:id="rId1"/>
@@ -276,26 +276,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="5" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="5" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="5" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,14 +697,14 @@
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -746,10 +746,10 @@
       <c r="D5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="20">
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -767,10 +767,10 @@
       <c r="D6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>0.20833333333333334</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="20">
         <v>0.14047453703703702</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -788,10 +788,10 @@
       <c r="D7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="20">
         <v>2.9178240740740741E-2</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -809,10 +809,12 @@
       <c r="D8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="16">
+        <v>8.6956018518518516E-2</v>
+      </c>
       <c r="G8" s="11" t="s">
         <v>25</v>
       </c>
@@ -864,18 +866,18 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="17">
         <f>SUM(E5:E13)</f>
         <v>0.37500000000000006</v>
       </c>
       <c r="F14" s="17">
         <f>SUM(F5:F13)</f>
-        <v>0.23076388888888888</v>
+        <v>0.31771990740740741</v>
       </c>
       <c r="G14" s="6"/>
     </row>
@@ -925,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,14 +950,14 @@
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -997,10 +999,10 @@
       <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>0.1875</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="20">
         <v>6.25E-2</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -1018,10 +1020,10 @@
       <c r="D6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="20">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="19">
         <v>6.9456018518518514E-2</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -1039,10 +1041,12 @@
       <c r="D7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="16">
+        <v>8.6956018518518516E-2</v>
+      </c>
       <c r="G7" s="11" t="s">
         <v>25</v>
       </c>
@@ -1112,18 +1116,18 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="17">
         <f>SUM(E5:E14)</f>
         <v>0.27083333333333331</v>
       </c>
       <c r="F15" s="17">
         <f>SUM(F5:F14)</f>
-        <v>0.13195601851851851</v>
+        <v>0.21891203703703704</v>
       </c>
       <c r="G15" s="6"/>
     </row>
@@ -1184,12 +1188,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
@@ -1210,39 +1214,39 @@
       <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="22">
         <f>SumEstJaneczek</f>
         <v>0.37500000000000006</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <f>SumActJaneczek</f>
-        <v>0.23076388888888888</v>
+        <v>0.31771990740740741</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="22">
         <f>SumEstMair</f>
         <v>0.27083333333333331</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <f>SumActMair</f>
-        <v>0.13195601851851851</v>
+        <v>0.21891203703703704</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="22">
         <f>SUM(SumEstJaneczek+SumEstMair)</f>
         <v>0.64583333333333337</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="23">
         <f>SUM(SumActJaneczek+SumActMair)</f>
-        <v>0.36271990740740739</v>
+        <v>0.53663194444444451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>